<commit_message>
Updated Sprint_Backlog with assigned tasks
</commit_message>
<xml_diff>
--- a/documentation/Sprint_Backlog_Burndown.xlsx
+++ b/documentation/Sprint_Backlog_Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/daf4c36fd6410f15/Desktop/JamesBridgesHW5_Sprint1/TextAdventureGame/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A620CB8D-31DF-4764-AA14-2152C40C01F3}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2885C487-3284-4422-97C9-AE3D6680D6C7}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3984" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Related User Story</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>James Bridges</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Brailey</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B7" sqref="B3:B7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1429,6 +1435,9 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -1442,6 +1451,9 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -1455,6 +1467,9 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
+      <c r="Q5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -1468,6 +1483,9 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
+      <c r="Q6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -1481,6 +1499,9 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+      <c r="Q7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -1494,6 +1515,9 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -1507,6 +1531,9 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -1520,6 +1547,9 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -1533,6 +1563,9 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
+      <c r="Q11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -1546,6 +1579,9 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
Added Location Reading From File
LocationReader takes file path from WorldManager in order to generate locations.
</commit_message>
<xml_diff>
--- a/documentation/Sprint_Backlog_Burndown.xlsx
+++ b/documentation/Sprint_Backlog_Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/daf4c36fd6410f15/Desktop/JamesBridgesHW5_Sprint1/TextAdventureGame/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lw00116\Desktop\Text Adventure James\TextAdventureGame\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2885C487-3284-4422-97C9-AE3D6680D6C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87110851-D776-430A-88F3-A6D516694A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Related User Story</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Brailey</t>
+  </si>
+  <si>
+    <t>Load Locations From File</t>
   </si>
 </sst>
 </file>
@@ -313,7 +316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1104,10 +1107,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1373,18 +1372,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:Q12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1421,7 +1420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1439,7 +1438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -1455,7 +1454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -1471,7 +1470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1487,7 +1486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -1503,7 +1502,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1519,7 +1518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>16</v>
@@ -1535,7 +1534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -1551,7 +1550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -1567,7 +1566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1583,7 +1582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>20</v>
@@ -1599,16 +1598,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1617,7 +1623,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1626,7 +1632,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1635,7 +1641,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1644,7 +1650,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1653,7 +1659,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1662,7 +1668,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1671,7 +1677,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1680,7 +1686,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1689,7 +1695,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1698,7 +1704,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1707,7 +1713,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1716,13 +1722,13 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="3">
         <f>SUM(C3:C26)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>

</xml_diff>

<commit_message>
Added NPC model class
NPC currently only has a description meant to identify it as being present in a specific location. None of the logic that directly connects an NPC to a location is implemented.
</commit_message>
<xml_diff>
--- a/documentation/Sprint_Backlog_Burndown.xlsx
+++ b/documentation/Sprint_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lw00116\Desktop\Text Adventure James\TextAdventureGame\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87110851-D776-430A-88F3-A6D516694A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA327131-9881-4C7B-84F7-57C45788E678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1372,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1444,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="C27" s="3">
         <f>SUM(C3:C26)</f>
-        <v>40</v>
+        <v>39.5</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>

</xml_diff>

<commit_message>
Added NPC To The World
NPC can be identified as being present in the world through the getDescription method of Location. Cannot be currently interacted with.
</commit_message>
<xml_diff>
--- a/documentation/Sprint_Backlog_Burndown.xlsx
+++ b/documentation/Sprint_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lw00116\Desktop\Text Adventure James\TextAdventureGame\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA327131-9881-4C7B-84F7-57C45788E678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E16EB18-F30A-42F9-85D5-6B6F3997B47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1373,7 +1373,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1444,7 +1444,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1460,7 +1460,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1492,7 +1492,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="C27" s="3">
         <f>SUM(C3:C26)</f>
-        <v>39.5</v>
+        <v>36.5</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>

</xml_diff>

<commit_message>
NPC Can Now Move
NPC can now move after being talked to with new Talk action. Note: Talking to NPC at their second location causes there to be multiple talk actions added to the location. Furthermore, rainy day tests for NPC setters not implemented.
</commit_message>
<xml_diff>
--- a/documentation/Sprint_Backlog_Burndown.xlsx
+++ b/documentation/Sprint_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lw00116\Desktop\Text Adventure James\TextAdventureGame\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E16EB18-F30A-42F9-85D5-6B6F3997B47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E5716F-AB7D-413E-99DB-8790F421BA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.5</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1373,7 +1373,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1444,7 +1444,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1476,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1492,7 +1492,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="C27" s="3">
         <f>SUM(C3:C26)</f>
-        <v>36.5</v>
+        <v>34.5</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>

</xml_diff>

<commit_message>
All NPC Functionality Implemented
NPC behavior is primarily handled with the GameManager. Give action added, which allows the npc to give feedback on the correct item. Once correct item is given, NPC will leave, take the item, and GameManager will connect entrance hall to exit. GameManager NPC functionality is not properly tested.
</commit_message>
<xml_diff>
--- a/documentation/Sprint_Backlog_Burndown.xlsx
+++ b/documentation/Sprint_Backlog_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lw00116\Desktop\Text Adventure James\TextAdventureGame\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E5716F-AB7D-413E-99DB-8790F421BA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA114AD-66EF-49C8-B17B-92CE4D60D5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1373,7 +1373,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1444,7 +1444,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1476,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1492,7 +1492,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="C27" s="3">
         <f>SUM(C3:C26)</f>
-        <v>34.5</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>

</xml_diff>